<commit_message>
Refactor and clean code, pageThree : ok
</commit_message>
<xml_diff>
--- a/Deuxième Question Tour1.xlsx
+++ b/Deuxième Question Tour1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>http://dbpedia.org/ontology/birthPlace</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>http://dbpedia.org/ontology/associateStar</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -488,6 +493,11 @@
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -512,6 +522,11 @@
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -532,6 +547,11 @@
           <t>http://dbpedia.org/resource/Windsor</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -550,6 +570,11 @@
       <c r="F5" t="inlineStr">
         <is>
           <t>http://dbpedia.org/resource/Berlin</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>nan</t>
         </is>
       </c>
     </row>

</xml_diff>